<commit_message>
made changes in the excel
</commit_message>
<xml_diff>
--- a/database/microfin_manager_db.xlsx
+++ b/database/microfin_manager_db.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\microfin-ug\manager\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\xampp\htdocs\microfin-ug\manager\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D5700F-1D4B-468B-B5B2-79871B91A59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8F08D5-09CA-44D8-B372-13927EC5B574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="253">
   <si>
     <t>org_name</t>
   </si>
@@ -802,6 +802,9 @@
   </si>
   <si>
     <t>Opening Balance for imports</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -890,7 +893,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -926,6 +929,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1206,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D276"/>
+  <dimension ref="A1:D277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
-      <selection activeCell="D224" sqref="D224"/>
+    <sheetView tabSelected="1" topLeftCell="A264" workbookViewId="0">
+      <selection activeCell="A277" sqref="A277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2622,6 +2626,11 @@
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" s="5" t="s">
         <v>250</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="19" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>